<commit_message>
updated with hashing notes
</commit_message>
<xml_diff>
--- a/DSA Solutions.xlsx
+++ b/DSA Solutions.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Problem-soln" sheetId="1" r:id="rId1"/>
+    <sheet name="NOTES" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Problem </t>
   </si>
@@ -45,13 +46,34 @@
   </si>
   <si>
     <t xml:space="preserve">Create an new array with size of maxium element . Loop over oriiginal array and increase count.  Based on question check whether to consider n or n-1 index. </t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>TOPIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hashing </t>
+  </si>
+  <si>
+    <t>Data can be hashed in the form of array /map to store their frequency or other data. For large Data hasing technique such as division hasing can be used. Like mod element with 10 and store in map of &lt;int,LinkedList&gt;  e.g 8-&gt; 8,18,28,38...</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/studio/problems/k-most-occurrent-numbers_625382?utm_source=striver&amp;utm_medium=website&amp;utm_campaign=a_zcoursetuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count min max frequency </t>
+  </si>
+  <si>
+    <t>hash as map. Set returun array vals as -1. Then loop over hashmap to get min and max frequency. In first itr set  array min max to first element . Bit tricky but easy.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +93,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -107,6 +137,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -390,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +449,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -430,11 +464,59 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="80.28515625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bubble Sort and solns
</commit_message>
<xml_diff>
--- a/DSA Solutions.xlsx
+++ b/DSA Solutions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Problem </t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>hash as map. Set returun array vals as -1. Then loop over hashmap to get min and max frequency. In first itr set  array min max to first element . Bit tricky but easy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selection sort </t>
+  </si>
+  <si>
+    <t>goal is with each iteration put smaller element in correct position. example for 5 4 3 2 solution will be 2 4 3 5 ,  2 3 4 5 Remember - find the minimal and swap</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/studio/problems/selection-sort_624469?utm_source=striver&amp;utm_medium=website&amp;utm_campaign=a_zcoursetuf</t>
+  </si>
+  <si>
+    <t>Bubble Sort</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/studio/problems/bubble-sort_624380?utm_source=striver&amp;utm_medium=website&amp;utm_campaign=a_zcoursetuf</t>
   </si>
 </sst>
 </file>
@@ -424,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,13 +493,41 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Check if array is sorted
</commit_message>
<xml_diff>
--- a/DSA Solutions.xlsx
+++ b/DSA Solutions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Problem </t>
   </si>
@@ -85,6 +85,19 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/studio/problems/bubble-sort_624380?utm_source=striver&amp;utm_medium=website&amp;utm_campaign=a_zcoursetuf</t>
+  </si>
+  <si>
+    <t>Insertion sort</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/studio/problems/insertion-sort_624381?utm_source=striver&amp;utm_medium=website&amp;utm_campaign=a_zcoursetuf&amp;leftPanelTab=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keep comparing every element with left elements , keep swapping until left is greater
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjcent swapping </t>
   </si>
 </sst>
 </file>
@@ -442,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +531,20 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -525,9 +552,10 @@
     <hyperlink ref="B5" r:id="rId2"/>
     <hyperlink ref="B9" r:id="rId3"/>
     <hyperlink ref="B10" r:id="rId4"/>
+    <hyperlink ref="B11" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>